<commit_message>
finalized all code cells, just need to add commenting
</commit_message>
<xml_diff>
--- a/finished_files/momentum_strategy.xlsx
+++ b/finished_files/momentum_strategy.xlsx
@@ -636,37 +636,37 @@
         <v>12</v>
       </c>
       <c r="B2" s="2">
-        <v>101.76</v>
+        <v>101.74</v>
       </c>
       <c r="C2" s="3">
         <v>192</v>
       </c>
       <c r="D2" s="4">
-        <v>0.46</v>
+        <v>0.4528</v>
       </c>
       <c r="E2" s="4">
-        <v>89.70297029702971</v>
+        <v>0.895049504950495</v>
       </c>
       <c r="F2" s="4">
-        <v>0.1802</v>
+        <v>0.184</v>
       </c>
       <c r="G2" s="4">
-        <v>86.33663366336634</v>
+        <v>0.8653465346534653</v>
       </c>
       <c r="H2" s="4">
-        <v>0.2463</v>
+        <v>0.2497</v>
       </c>
       <c r="I2" s="4">
-        <v>78.41584158415841</v>
+        <v>0.794059405940594</v>
       </c>
       <c r="J2" s="4">
-        <v>0.1004</v>
+        <v>0.09760000000000001</v>
       </c>
       <c r="K2" s="4">
-        <v>68.11881188118812</v>
+        <v>0.6633663366336634</v>
       </c>
       <c r="L2" s="3">
-        <v>80.64356435643565</v>
+        <v>0.8044554455445544</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -674,37 +674,37 @@
         <v>13</v>
       </c>
       <c r="B3" s="2">
-        <v>13.56</v>
+        <v>13.975</v>
       </c>
       <c r="C3" s="3">
-        <v>1446</v>
+        <v>1403</v>
       </c>
       <c r="D3" s="4">
-        <v>-0.5697</v>
+        <v>-0.5472</v>
       </c>
       <c r="E3" s="4">
-        <v>2.178217821782178</v>
+        <v>0.02772277227722772</v>
       </c>
       <c r="F3" s="4">
-        <v>-0.5673</v>
+        <v>-0.5655</v>
       </c>
       <c r="G3" s="4">
-        <v>1.584158415841584</v>
+        <v>0.01782178217821782</v>
       </c>
       <c r="H3" s="4">
-        <v>0.3725</v>
+        <v>0.3764</v>
       </c>
       <c r="I3" s="4">
-        <v>92.87128712871286</v>
+        <v>0.9267326732673267</v>
       </c>
       <c r="J3" s="4">
-        <v>0.096</v>
+        <v>0.098</v>
       </c>
       <c r="K3" s="4">
-        <v>65.74257425742574</v>
+        <v>0.6653465346534654</v>
       </c>
       <c r="L3" s="3">
-        <v>40.59405940594059</v>
+        <v>0.4094059405940594</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -712,37 +712,37 @@
         <v>14</v>
       </c>
       <c r="B4" s="2">
-        <v>156.89</v>
+        <v>158.776</v>
       </c>
       <c r="C4" s="3">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4" s="4">
-        <v>0.0553</v>
+        <v>0.0563</v>
       </c>
       <c r="E4" s="4">
-        <v>54.45544554455446</v>
+        <v>0.5465346534653466</v>
       </c>
       <c r="F4" s="4">
-        <v>0.1482</v>
+        <v>0.1447</v>
       </c>
       <c r="G4" s="4">
-        <v>81.98019801980197</v>
+        <v>0.8138613861386139</v>
       </c>
       <c r="H4" s="4">
-        <v>0.277</v>
+        <v>0.2754</v>
       </c>
       <c r="I4" s="4">
-        <v>83.16831683168317</v>
+        <v>0.8198019801980198</v>
       </c>
       <c r="J4" s="4">
-        <v>0.1139</v>
+        <v>0.1141</v>
       </c>
       <c r="K4" s="4">
-        <v>73.26732673267327</v>
+        <v>0.7306930693069308</v>
       </c>
       <c r="L4" s="3">
-        <v>73.21782178217822</v>
+        <v>0.7277227722772277</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -750,37 +750,37 @@
         <v>15</v>
       </c>
       <c r="B5" s="2">
-        <v>456.43</v>
+        <v>465.87</v>
       </c>
       <c r="C5" s="3">
         <v>42</v>
       </c>
       <c r="D5" s="4">
-        <v>1.281</v>
+        <v>1.29</v>
       </c>
       <c r="E5" s="4">
-        <v>99.20792079207921</v>
+        <v>0.9920792079207921</v>
       </c>
       <c r="F5" s="4">
-        <v>0.404</v>
+        <v>0.4051</v>
       </c>
       <c r="G5" s="4">
-        <v>95.64356435643565</v>
+        <v>0.9564356435643565</v>
       </c>
       <c r="H5" s="4">
-        <v>0.4714</v>
+        <v>0.4858</v>
       </c>
       <c r="I5" s="4">
-        <v>97.42574257425743</v>
+        <v>0.9782178217821782</v>
       </c>
       <c r="J5" s="4">
-        <v>0.1987</v>
+        <v>0.1972</v>
       </c>
       <c r="K5" s="4">
-        <v>94.25742574257426</v>
+        <v>0.9405940594059407</v>
       </c>
       <c r="L5" s="3">
-        <v>96.63366336633663</v>
+        <v>0.9668316831683168</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -788,37 +788,37 @@
         <v>16</v>
       </c>
       <c r="B6" s="2">
-        <v>96.73</v>
+        <v>95.39</v>
       </c>
       <c r="C6" s="3">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D6" s="4">
-        <v>0.4527</v>
+        <v>0.4463</v>
       </c>
       <c r="E6" s="4">
-        <v>89.3069306930693</v>
+        <v>0.887128712871287</v>
       </c>
       <c r="F6" s="4">
-        <v>0.007</v>
+        <v>0.0069</v>
       </c>
       <c r="G6" s="4">
-        <v>64.35643564356435</v>
+        <v>0.6435643564356436</v>
       </c>
       <c r="H6" s="4">
-        <v>0.1041</v>
+        <v>0.1064</v>
       </c>
       <c r="I6" s="4">
-        <v>43.96039603960396</v>
+        <v>0.4514851485148514</v>
       </c>
       <c r="J6" s="4">
-        <v>-0.0678</v>
+        <v>-0.067</v>
       </c>
       <c r="K6" s="4">
-        <v>3.762376237623762</v>
+        <v>0.03762376237623762</v>
       </c>
       <c r="L6" s="3">
-        <v>50.34653465346535</v>
+        <v>0.504950495049505</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -826,37 +826,37 @@
         <v>17</v>
       </c>
       <c r="B7" s="2">
-        <v>106.6</v>
+        <v>103.71</v>
       </c>
       <c r="C7" s="3">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D7" s="4">
-        <v>0.1926</v>
+        <v>0.196</v>
       </c>
       <c r="E7" s="4">
-        <v>69.9009900990099</v>
+        <v>0.704950495049505</v>
       </c>
       <c r="F7" s="4">
-        <v>0.1105</v>
+        <v>0.1107</v>
       </c>
       <c r="G7" s="4">
-        <v>77.42574257425743</v>
+        <v>0.7762376237623763</v>
       </c>
       <c r="H7" s="4">
-        <v>0.1551</v>
+        <v>0.1511</v>
       </c>
       <c r="I7" s="4">
-        <v>57.82178217821782</v>
+        <v>0.5683168316831683</v>
       </c>
       <c r="J7" s="4">
-        <v>0.0406</v>
+        <v>0.0394</v>
       </c>
       <c r="K7" s="4">
-        <v>33.86138613861386</v>
+        <v>0.3326732673267327</v>
       </c>
       <c r="L7" s="3">
-        <v>59.75247524752476</v>
+        <v>0.5955445544554455</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -864,37 +864,37 @@
         <v>18</v>
       </c>
       <c r="B8" s="2">
-        <v>317.78</v>
+        <v>314.533</v>
       </c>
       <c r="C8" s="3">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D8" s="4">
-        <v>0.6424</v>
+        <v>0.6482</v>
       </c>
       <c r="E8" s="4">
-        <v>96.23762376237623</v>
+        <v>0.9663366336633663</v>
       </c>
       <c r="F8" s="4">
-        <v>0.6657999999999999</v>
+        <v>0.6929</v>
       </c>
       <c r="G8" s="4">
-        <v>99.00990099009901</v>
+        <v>0.9920792079207921</v>
       </c>
       <c r="H8" s="4">
-        <v>0.6752</v>
+        <v>0.654</v>
       </c>
       <c r="I8" s="4">
-        <v>99.60396039603961</v>
+        <v>0.9940594059405941</v>
       </c>
       <c r="J8" s="4">
-        <v>0.1804</v>
+        <v>0.1761</v>
       </c>
       <c r="K8" s="4">
-        <v>91.28712871287129</v>
+        <v>0.9108910891089108</v>
       </c>
       <c r="L8" s="3">
-        <v>96.53465346534654</v>
+        <v>0.9658415841584158</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -902,37 +902,37 @@
         <v>19</v>
       </c>
       <c r="B9" s="2">
-        <v>105.54</v>
+        <v>102.45</v>
       </c>
       <c r="C9" s="3">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D9" s="4">
-        <v>0.1985</v>
+        <v>0.1972</v>
       </c>
       <c r="E9" s="4">
-        <v>70.6930693069307</v>
+        <v>0.706930693069307</v>
       </c>
       <c r="F9" s="4">
-        <v>0.159</v>
+        <v>0.154</v>
       </c>
       <c r="G9" s="4">
-        <v>83.16831683168317</v>
+        <v>0.8277227722772277</v>
       </c>
       <c r="H9" s="4">
-        <v>0.08</v>
+        <v>0.081</v>
       </c>
       <c r="I9" s="4">
-        <v>36.43564356435643</v>
+        <v>0.3663366336633663</v>
       </c>
       <c r="J9" s="4">
-        <v>0.0958</v>
+        <v>0.0994</v>
       </c>
       <c r="K9" s="4">
-        <v>65.54455445544555</v>
+        <v>0.6712871287128713</v>
       </c>
       <c r="L9" s="3">
-        <v>63.96039603960396</v>
+        <v>0.6430693069306931</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -940,37 +940,37 @@
         <v>20</v>
       </c>
       <c r="B10" s="2">
-        <v>242.77</v>
+        <v>235.64</v>
       </c>
       <c r="C10" s="3">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D10" s="4">
-        <v>0.235</v>
+        <v>0.231</v>
       </c>
       <c r="E10" s="4">
-        <v>74.25742574257426</v>
+        <v>0.7366336633663366</v>
       </c>
       <c r="F10" s="4">
-        <v>0.0978</v>
+        <v>0.0985</v>
       </c>
       <c r="G10" s="4">
-        <v>76.03960396039604</v>
+        <v>0.7603960396039604</v>
       </c>
       <c r="H10" s="4">
-        <v>0.2417</v>
+        <v>0.2473</v>
       </c>
       <c r="I10" s="4">
-        <v>77.02970297029702</v>
+        <v>0.7881188118811882</v>
       </c>
       <c r="J10" s="4">
-        <v>0.07149999999999999</v>
+        <v>0.0704</v>
       </c>
       <c r="K10" s="4">
-        <v>50.0990099009901</v>
+        <v>0.495049504950495</v>
       </c>
       <c r="L10" s="3">
-        <v>69.35643564356435</v>
+        <v>0.695049504950495</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -978,37 +978,37 @@
         <v>21</v>
       </c>
       <c r="B11" s="2">
-        <v>460.92</v>
+        <v>464.39</v>
       </c>
       <c r="C11" s="3">
         <v>42</v>
       </c>
       <c r="D11" s="4">
-        <v>0.5611</v>
+        <v>0.5605</v>
       </c>
       <c r="E11" s="4">
-        <v>94.25742574257426</v>
+        <v>0.9425742574257425</v>
       </c>
       <c r="F11" s="4">
-        <v>0.237</v>
+        <v>0.234</v>
       </c>
       <c r="G11" s="4">
-        <v>90.0990099009901</v>
+        <v>0.899009900990099</v>
       </c>
       <c r="H11" s="4">
-        <v>0.2294</v>
+        <v>0.2302</v>
       </c>
       <c r="I11" s="4">
-        <v>74.25742574257426</v>
+        <v>0.7504950495049505</v>
       </c>
       <c r="J11" s="4">
         <v>0.0005</v>
       </c>
       <c r="K11" s="4">
-        <v>18.61386138613861</v>
+        <v>0.1861386138613861</v>
       </c>
       <c r="L11" s="3">
-        <v>69.3069306930693</v>
+        <v>0.6945544554455445</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1016,37 +1016,37 @@
         <v>22</v>
       </c>
       <c r="B12" s="2">
-        <v>117.36</v>
+        <v>120.2</v>
       </c>
       <c r="C12" s="3">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D12" s="4">
-        <v>0.0605</v>
+        <v>0.0619</v>
       </c>
       <c r="E12" s="4">
-        <v>55.44554455445545</v>
+        <v>0.5544554455445545</v>
       </c>
       <c r="F12" s="4">
-        <v>0.0366</v>
+        <v>0.0371</v>
       </c>
       <c r="G12" s="4">
-        <v>68.31683168316832</v>
+        <v>0.6831683168316832</v>
       </c>
       <c r="H12" s="4">
-        <v>0.0978</v>
+        <v>0.0968</v>
       </c>
       <c r="I12" s="4">
-        <v>41.38613861386138</v>
+        <v>0.4099009900990099</v>
       </c>
       <c r="J12" s="4">
-        <v>-0.053</v>
+        <v>-0.0538</v>
       </c>
       <c r="K12" s="4">
-        <v>6.534653465346534</v>
+        <v>0.0594059405940594</v>
       </c>
       <c r="L12" s="3">
-        <v>42.92079207920792</v>
+        <v>0.4267326732673268</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1054,37 +1054,37 @@
         <v>23</v>
       </c>
       <c r="B13" s="2">
-        <v>44.81</v>
+        <v>44.45</v>
       </c>
       <c r="C13" s="3">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="D13" s="4">
-        <v>0.1854</v>
+        <v>0.1874</v>
       </c>
       <c r="E13" s="4">
-        <v>68.71287128712871</v>
+        <v>0.6910891089108911</v>
       </c>
       <c r="F13" s="4">
-        <v>-0.0375</v>
+        <v>-0.0382</v>
       </c>
       <c r="G13" s="4">
-        <v>55.64356435643565</v>
+        <v>0.5544554455445545</v>
       </c>
       <c r="H13" s="4">
-        <v>0.2788</v>
+        <v>0.2799</v>
       </c>
       <c r="I13" s="4">
-        <v>83.36633663366337</v>
+        <v>0.8297029702970298</v>
       </c>
       <c r="J13" s="4">
-        <v>0.1232</v>
+        <v>0.1263</v>
       </c>
       <c r="K13" s="4">
-        <v>78.01980198019803</v>
+        <v>0.7881188118811882</v>
       </c>
       <c r="L13" s="3">
-        <v>71.43564356435644</v>
+        <v>0.7158415841584159</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1092,37 +1092,37 @@
         <v>24</v>
       </c>
       <c r="B14" s="2">
-        <v>138.42</v>
+        <v>141.4</v>
       </c>
       <c r="C14" s="3">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D14" s="4">
-        <v>-0.163</v>
+        <v>-0.165</v>
       </c>
       <c r="E14" s="4">
-        <v>28.91089108910891</v>
+        <v>0.2891089108910891</v>
       </c>
       <c r="F14" s="4">
-        <v>-0.2385</v>
+        <v>-0.24</v>
       </c>
       <c r="G14" s="4">
-        <v>26.53465346534653</v>
+        <v>0.2633663366336634</v>
       </c>
       <c r="H14" s="4">
-        <v>-0.0688</v>
+        <v>-0.0689</v>
       </c>
       <c r="I14" s="4">
-        <v>6.138613861386139</v>
+        <v>0.0594059405940594</v>
       </c>
       <c r="J14" s="4">
-        <v>-0.064</v>
+        <v>-0.0633</v>
       </c>
       <c r="K14" s="4">
-        <v>4.752475247524752</v>
+        <v>0.04950495049504951</v>
       </c>
       <c r="L14" s="3">
-        <v>16.58415841584159</v>
+        <v>0.1653465346534654</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1130,37 +1130,37 @@
         <v>25</v>
       </c>
       <c r="B15" s="2">
-        <v>245.87</v>
+        <v>241.7</v>
       </c>
       <c r="C15" s="3">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D15" s="4">
-        <v>0.6612</v>
+        <v>0.6388</v>
       </c>
       <c r="E15" s="4">
-        <v>96.83168316831683</v>
+        <v>0.9643564356435644</v>
       </c>
       <c r="F15" s="4">
-        <v>0.1438</v>
+        <v>0.1478</v>
       </c>
       <c r="G15" s="4">
-        <v>81.78217821782178</v>
+        <v>0.8198019801980198</v>
       </c>
       <c r="H15" s="4">
-        <v>0.2845</v>
+        <v>0.2948</v>
       </c>
       <c r="I15" s="4">
-        <v>85.14851485148515</v>
+        <v>0.8554455445544555</v>
       </c>
       <c r="J15" s="4">
-        <v>-0.0116</v>
+        <v>-0.0117</v>
       </c>
       <c r="K15" s="4">
-        <v>14.45544554455446</v>
+        <v>0.1445544554455446</v>
       </c>
       <c r="L15" s="3">
-        <v>69.55445544554455</v>
+        <v>0.6960396039603961</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1168,37 +1168,37 @@
         <v>26</v>
       </c>
       <c r="B16" s="2">
-        <v>84.48999999999999</v>
+        <v>83.75</v>
       </c>
       <c r="C16" s="3">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D16" s="4">
-        <v>0.09379999999999999</v>
+        <v>0.0948</v>
       </c>
       <c r="E16" s="4">
-        <v>60.19801980198019</v>
+        <v>0.6079207920792079</v>
       </c>
       <c r="F16" s="4">
         <v>-0.017</v>
       </c>
       <c r="G16" s="4">
-        <v>58.41584158415841</v>
+        <v>0.5841584158415841</v>
       </c>
       <c r="H16" s="4">
-        <v>0.1815</v>
+        <v>0.185</v>
       </c>
       <c r="I16" s="4">
-        <v>65.54455445544555</v>
+        <v>0.6712871287128713</v>
       </c>
       <c r="J16" s="4">
-        <v>0.1222</v>
+        <v>0.1214</v>
       </c>
       <c r="K16" s="4">
-        <v>77.02970297029702</v>
+        <v>0.7663366336633664</v>
       </c>
       <c r="L16" s="3">
-        <v>65.29702970297029</v>
+        <v>0.6574257425742575</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1206,37 +1206,37 @@
         <v>27</v>
       </c>
       <c r="B17" s="2">
-        <v>88.59999999999999</v>
+        <v>89.73</v>
       </c>
       <c r="C17" s="3">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D17" s="4">
         <v>-0.036</v>
       </c>
       <c r="E17" s="4">
-        <v>42.97029702970297</v>
+        <v>0.4297029702970297</v>
       </c>
       <c r="F17" s="4">
-        <v>-0.15</v>
+        <v>-0.151</v>
       </c>
       <c r="G17" s="4">
-        <v>37.82178217821782</v>
+        <v>0.3782178217821782</v>
       </c>
       <c r="H17" s="4">
-        <v>0.1029</v>
+        <v>0.1047</v>
       </c>
       <c r="I17" s="4">
-        <v>43.76237623762376</v>
+        <v>0.4435643564356435</v>
       </c>
       <c r="J17" s="4">
-        <v>0.0515</v>
+        <v>0.0518</v>
       </c>
       <c r="K17" s="4">
-        <v>38.01980198019802</v>
+        <v>0.3801980198019802</v>
       </c>
       <c r="L17" s="3">
-        <v>40.64356435643565</v>
+        <v>0.4079207920792079</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1244,37 +1244,37 @@
         <v>28</v>
       </c>
       <c r="B18" s="2">
-        <v>17.48</v>
+        <v>17.568</v>
       </c>
       <c r="C18" s="3">
-        <v>1121</v>
+        <v>1116</v>
       </c>
       <c r="D18" s="4">
-        <v>0.0951</v>
+        <v>0.0958</v>
       </c>
       <c r="E18" s="4">
-        <v>60.79207920792079</v>
+        <v>0.6118811881188119</v>
       </c>
       <c r="F18" s="4">
-        <v>-0.1656</v>
+        <v>-0.1666</v>
       </c>
       <c r="G18" s="4">
-        <v>35.64356435643565</v>
+        <v>0.3564356435643565</v>
       </c>
       <c r="H18" s="4">
-        <v>0.4307</v>
+        <v>0.4181</v>
       </c>
       <c r="I18" s="4">
-        <v>95.84158415841584</v>
+        <v>0.9544554455445545</v>
       </c>
       <c r="J18" s="4">
-        <v>0.2218</v>
+        <v>0.2167</v>
       </c>
       <c r="K18" s="4">
-        <v>96.83168316831683</v>
+        <v>0.9623762376237623</v>
       </c>
       <c r="L18" s="3">
-        <v>72.27722772277228</v>
+        <v>0.7212871287128713</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1282,37 +1282,37 @@
         <v>29</v>
       </c>
       <c r="B19" s="2">
-        <v>36.63</v>
+        <v>38.04</v>
       </c>
       <c r="C19" s="3">
-        <v>535</v>
+        <v>515</v>
       </c>
       <c r="D19" s="4">
-        <v>-0.3045</v>
+        <v>-0.2998</v>
       </c>
       <c r="E19" s="4">
-        <v>14.65346534653465</v>
+        <v>0.1584158415841584</v>
       </c>
       <c r="F19" s="4">
-        <v>-0.31</v>
+        <v>-0.33</v>
       </c>
       <c r="G19" s="4">
-        <v>17.22772277227723</v>
+        <v>0.1485148514851485</v>
       </c>
       <c r="H19" s="4">
-        <v>0.0185</v>
+        <v>0.0186</v>
       </c>
       <c r="I19" s="4">
-        <v>21.18811881188119</v>
+        <v>0.2118811881188119</v>
       </c>
       <c r="J19" s="4">
-        <v>0.0549</v>
+        <v>0.0568</v>
       </c>
       <c r="K19" s="4">
-        <v>40</v>
+        <v>0.4099009900990099</v>
       </c>
       <c r="L19" s="3">
-        <v>23.26732673267327</v>
+        <v>0.2321782178217822</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1320,37 +1320,37 @@
         <v>30</v>
       </c>
       <c r="B20" s="2">
-        <v>31.45</v>
+        <v>31.62</v>
       </c>
       <c r="C20" s="3">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D20" s="4">
-        <v>-0.464652</v>
+        <v>-0.476271</v>
       </c>
       <c r="E20" s="4">
-        <v>4.752475247524752</v>
+        <v>0.04752475247524753</v>
       </c>
       <c r="F20" s="4">
-        <v>-0.43505</v>
+        <v>-0.44938</v>
       </c>
       <c r="G20" s="4">
-        <v>6.138613861386139</v>
+        <v>0.05742574257425742</v>
       </c>
       <c r="H20" s="4">
-        <v>0.110944</v>
+        <v>0.113528</v>
       </c>
       <c r="I20" s="4">
-        <v>46.33663366336634</v>
+        <v>0.4693069306930693</v>
       </c>
       <c r="J20" s="4">
-        <v>0.027474</v>
+        <v>0.028053</v>
       </c>
       <c r="K20" s="4">
-        <v>28.31683168316832</v>
+        <v>0.2851485148514852</v>
       </c>
       <c r="L20" s="3">
-        <v>21.38613861386139</v>
+        <v>0.2148514851485149</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1358,37 +1358,37 @@
         <v>31</v>
       </c>
       <c r="B21" s="2">
-        <v>37.55</v>
+        <v>38.92</v>
       </c>
       <c r="C21" s="3">
-        <v>522</v>
+        <v>503</v>
       </c>
       <c r="D21" s="4">
-        <v>-0.278654</v>
+        <v>-0.277819</v>
       </c>
       <c r="E21" s="4">
-        <v>17.62376237623763</v>
+        <v>0.1782178217821782</v>
       </c>
       <c r="F21" s="4">
-        <v>-0.317678</v>
+        <v>-0.325533</v>
       </c>
       <c r="G21" s="4">
-        <v>16.03960396039604</v>
+        <v>0.1564356435643564</v>
       </c>
       <c r="H21" s="4">
-        <v>-0.021708</v>
+        <v>-0.02203</v>
       </c>
       <c r="I21" s="4">
-        <v>13.46534653465346</v>
+        <v>0.1346534653465347</v>
       </c>
       <c r="J21" s="4">
-        <v>-0.010713</v>
+        <v>-0.010423</v>
       </c>
       <c r="K21" s="4">
-        <v>15.04950495049505</v>
+        <v>0.1504950495049505</v>
       </c>
       <c r="L21" s="3">
-        <v>15.54455445544554</v>
+        <v>0.1549504950495049</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1396,37 +1396,37 @@
         <v>32</v>
       </c>
       <c r="B22" s="2">
-        <v>123.16</v>
+        <v>127.54</v>
       </c>
       <c r="C22" s="3">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D22" s="4">
-        <v>0.02394</v>
+        <v>0.02376</v>
       </c>
       <c r="E22" s="4">
-        <v>51.68316831683168</v>
+        <v>0.5188118811881188</v>
       </c>
       <c r="F22" s="4">
-        <v>-0.109871</v>
+        <v>-0.109145</v>
       </c>
       <c r="G22" s="4">
-        <v>43.56435643564357</v>
+        <v>0.4376237623762376</v>
       </c>
       <c r="H22" s="4">
-        <v>0.245076</v>
+        <v>0.237635</v>
       </c>
       <c r="I22" s="4">
-        <v>78.21782178217822</v>
+        <v>0.7643564356435644</v>
       </c>
       <c r="J22" s="4">
-        <v>0.220317</v>
+        <v>0.219625</v>
       </c>
       <c r="K22" s="4">
-        <v>96.43564356435644</v>
+        <v>0.9643564356435644</v>
       </c>
       <c r="L22" s="3">
-        <v>67.47524752475248</v>
+        <v>0.6712871287128713</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1434,37 +1434,37 @@
         <v>33</v>
       </c>
       <c r="B23" s="2">
-        <v>109.65</v>
+        <v>111.37</v>
       </c>
       <c r="C23" s="3">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D23" s="4">
-        <v>0.191342</v>
+        <v>0.187816</v>
       </c>
       <c r="E23" s="4">
-        <v>69.5049504950495</v>
+        <v>0.693069306930693</v>
       </c>
       <c r="F23" s="4">
-        <v>0.000293</v>
+        <v>0.000286</v>
       </c>
       <c r="G23" s="4">
-        <v>62.37623762376238</v>
+        <v>0.6217821782178218</v>
       </c>
       <c r="H23" s="4">
-        <v>0.23844</v>
+        <v>0.247092</v>
       </c>
       <c r="I23" s="4">
-        <v>76.43564356435644</v>
+        <v>0.7861386138613861</v>
       </c>
       <c r="J23" s="4">
-        <v>0.08695</v>
+        <v>0.08703900000000001</v>
       </c>
       <c r="K23" s="4">
-        <v>59.20792079207921</v>
+        <v>0.5980198019801981</v>
       </c>
       <c r="L23" s="3">
-        <v>66.88118811881188</v>
+        <v>0.6747524752475247</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1472,37 +1472,37 @@
         <v>34</v>
       </c>
       <c r="B24" s="2">
-        <v>110.36</v>
+        <v>112.54</v>
       </c>
       <c r="C24" s="3">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D24" s="4">
-        <v>0.23523</v>
+        <v>0.236877</v>
       </c>
       <c r="E24" s="4">
-        <v>74.45544554455445</v>
+        <v>0.7465346534653466</v>
       </c>
       <c r="F24" s="4">
-        <v>0.14154</v>
+        <v>0.14672</v>
       </c>
       <c r="G24" s="4">
-        <v>81.18811881188118</v>
+        <v>0.8178217821782178</v>
       </c>
       <c r="H24" s="4">
-        <v>0.08351699999999999</v>
+        <v>0.07983</v>
       </c>
       <c r="I24" s="4">
-        <v>37.62376237623762</v>
+        <v>0.3623762376237624</v>
       </c>
       <c r="J24" s="4">
-        <v>-0.03153</v>
+        <v>-0.03169</v>
       </c>
       <c r="K24" s="4">
-        <v>8.712871287128714</v>
+        <v>0.08712871287128714</v>
       </c>
       <c r="L24" s="3">
-        <v>50.49504950495049</v>
+        <v>0.5034653465346535</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1510,37 +1510,37 @@
         <v>35</v>
       </c>
       <c r="B25" s="2">
-        <v>86.59</v>
+        <v>88.29000000000001</v>
       </c>
       <c r="C25" s="3">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D25" s="4">
-        <v>0.152</v>
+        <v>0.15</v>
       </c>
       <c r="E25" s="4">
-        <v>66.13861386138613</v>
+        <v>0.6613861386138613</v>
       </c>
       <c r="F25" s="4">
-        <v>0.014692</v>
+        <v>0.014339</v>
       </c>
       <c r="G25" s="4">
-        <v>65.34653465346534</v>
+        <v>0.6534653465346534</v>
       </c>
       <c r="H25" s="4">
-        <v>0.319267</v>
+        <v>0.317456</v>
       </c>
       <c r="I25" s="4">
-        <v>87.72277227722772</v>
+        <v>0.8752475247524752</v>
       </c>
       <c r="J25" s="4">
-        <v>0.08533300000000001</v>
+        <v>0.08436399999999999</v>
       </c>
       <c r="K25" s="4">
-        <v>58.41584158415841</v>
+        <v>0.5821782178217823</v>
       </c>
       <c r="L25" s="3">
-        <v>69.4059405940594</v>
+        <v>0.693069306930693</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1548,37 +1548,37 @@
         <v>36</v>
       </c>
       <c r="B26" s="2">
-        <v>316.86</v>
+        <v>308.13</v>
       </c>
       <c r="C26" s="3">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D26" s="4">
-        <v>0.64296</v>
+        <v>0.62727</v>
       </c>
       <c r="E26" s="4">
-        <v>96.43564356435644</v>
+        <v>0.9603960396039604</v>
       </c>
       <c r="F26" s="4">
-        <v>0.187598</v>
+        <v>0.189242</v>
       </c>
       <c r="G26" s="4">
-        <v>87.12871287128714</v>
+        <v>0.8732673267326733</v>
       </c>
       <c r="H26" s="4">
-        <v>0.45704</v>
+        <v>0.46124</v>
       </c>
       <c r="I26" s="4">
-        <v>96.63366336633663</v>
+        <v>0.9683168316831683</v>
       </c>
       <c r="J26" s="4">
-        <v>0.099831</v>
+        <v>0.099149</v>
       </c>
       <c r="K26" s="4">
-        <v>67.72277227722772</v>
+        <v>0.6693069306930692</v>
       </c>
       <c r="L26" s="3">
-        <v>86.98019801980197</v>
+        <v>0.8678217821782178</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1586,37 +1586,37 @@
         <v>37</v>
       </c>
       <c r="B27" s="2">
-        <v>36.68</v>
+        <v>37.43</v>
       </c>
       <c r="C27" s="3">
-        <v>534</v>
+        <v>523</v>
       </c>
       <c r="D27" s="4">
-        <v>-0.435897</v>
+        <v>-0.448806</v>
       </c>
       <c r="E27" s="4">
-        <v>6.138613861386139</v>
+        <v>0.05346534653465347</v>
       </c>
       <c r="F27" s="4">
-        <v>-0.441817</v>
+        <v>-0.441789</v>
       </c>
       <c r="G27" s="4">
-        <v>5.742574257425742</v>
+        <v>0.06138613861386139</v>
       </c>
       <c r="H27" s="4">
-        <v>0.224654</v>
+        <v>0.223425</v>
       </c>
       <c r="I27" s="4">
-        <v>73.66336633663366</v>
+        <v>0.7326732673267327</v>
       </c>
       <c r="J27" s="4">
-        <v>0.009783</v>
+        <v>0.009856999999999999</v>
       </c>
       <c r="K27" s="4">
-        <v>21.78217821782178</v>
+        <v>0.2198019801980198</v>
       </c>
       <c r="L27" s="3">
-        <v>26.83168316831683</v>
+        <v>0.2668316831683168</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1624,37 +1624,37 @@
         <v>38</v>
       </c>
       <c r="B28" s="2">
-        <v>100.12</v>
+        <v>98.60299999999999</v>
       </c>
       <c r="C28" s="3">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D28" s="4">
-        <v>-0.081524</v>
+        <v>-0.08168</v>
       </c>
       <c r="E28" s="4">
-        <v>37.22772277227723</v>
+        <v>0.3722772277227723</v>
       </c>
       <c r="F28" s="4">
-        <v>-0.223888</v>
+        <v>-0.22292</v>
       </c>
       <c r="G28" s="4">
-        <v>28.71287128712871</v>
+        <v>0.2851485148514852</v>
       </c>
       <c r="H28" s="4">
-        <v>-0.039149</v>
+        <v>-0.039639</v>
       </c>
       <c r="I28" s="4">
-        <v>10.2970297029703</v>
+        <v>0.102970297029703</v>
       </c>
       <c r="J28" s="4">
-        <v>0.098786</v>
+        <v>0.102128</v>
       </c>
       <c r="K28" s="4">
-        <v>67.32673267326733</v>
+        <v>0.6910891089108911</v>
       </c>
       <c r="L28" s="3">
-        <v>35.89108910891089</v>
+        <v>0.3628712871287129</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1662,37 +1662,37 @@
         <v>39</v>
       </c>
       <c r="B29" s="2">
-        <v>102.28</v>
+        <v>101.88</v>
       </c>
       <c r="C29" s="3">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D29" s="4">
-        <v>0.010015</v>
+        <v>0.010044</v>
       </c>
       <c r="E29" s="4">
-        <v>49.10891089108911</v>
+        <v>0.4910891089108911</v>
       </c>
       <c r="F29" s="4">
-        <v>-0.276129</v>
+        <v>-0.271031</v>
       </c>
       <c r="G29" s="4">
-        <v>21.78217821782178</v>
+        <v>0.2277227722772277</v>
       </c>
       <c r="H29" s="4">
-        <v>-0.02174</v>
+        <v>-0.022143</v>
       </c>
       <c r="I29" s="4">
-        <v>13.26732673267327</v>
+        <v>0.1326732673267327</v>
       </c>
       <c r="J29" s="4">
-        <v>-0.024075</v>
+        <v>-0.023515</v>
       </c>
       <c r="K29" s="4">
-        <v>9.900990099009901</v>
+        <v>0.09900990099009901</v>
       </c>
       <c r="L29" s="3">
-        <v>23.51485148514852</v>
+        <v>0.2376237623762376</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1700,37 +1700,37 @@
         <v>40</v>
       </c>
       <c r="B30" s="2">
-        <v>105.56</v>
+        <v>105.267</v>
       </c>
       <c r="C30" s="3">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D30" s="4">
-        <v>-0.079391</v>
+        <v>-0.080772</v>
       </c>
       <c r="E30" s="4">
-        <v>37.62376237623762</v>
+        <v>0.3762376237623762</v>
       </c>
       <c r="F30" s="4">
-        <v>0.02347</v>
+        <v>0.02265</v>
       </c>
       <c r="G30" s="4">
-        <v>66.73267326732673</v>
+        <v>0.6673267326732674</v>
       </c>
       <c r="H30" s="4">
-        <v>0.061874</v>
+        <v>0.06116</v>
       </c>
       <c r="I30" s="4">
-        <v>32.07920792079208</v>
+        <v>0.3128712871287129</v>
       </c>
       <c r="J30" s="4">
-        <v>-0.04373</v>
+        <v>-0.044206</v>
       </c>
       <c r="K30" s="4">
-        <v>7.326732673267327</v>
+        <v>0.07326732673267328</v>
       </c>
       <c r="L30" s="3">
-        <v>35.94059405940594</v>
+        <v>0.3574257425742574</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1738,37 +1738,37 @@
         <v>41</v>
       </c>
       <c r="B31" s="2">
-        <v>65.70999999999999</v>
+        <v>67.16</v>
       </c>
       <c r="C31" s="3">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="D31" s="4">
-        <v>0.335622</v>
+        <v>0.330314</v>
       </c>
       <c r="E31" s="4">
-        <v>82.77227722772277</v>
+        <v>0.8237623762376238</v>
       </c>
       <c r="F31" s="4">
-        <v>0.010549</v>
+        <v>0.010768</v>
       </c>
       <c r="G31" s="4">
-        <v>64.75247524752476</v>
+        <v>0.6495049504950495</v>
       </c>
       <c r="H31" s="4">
-        <v>0.186017</v>
+        <v>0.182597</v>
       </c>
       <c r="I31" s="4">
-        <v>67.72277227722772</v>
+        <v>0.6633663366336634</v>
       </c>
       <c r="J31" s="4">
-        <v>0.012801</v>
+        <v>0.013146</v>
       </c>
       <c r="K31" s="4">
-        <v>23.36633663366337</v>
+        <v>0.2376237623762376</v>
       </c>
       <c r="L31" s="3">
-        <v>59.65346534653465</v>
+        <v>0.5935643564356436</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1776,37 +1776,37 @@
         <v>42</v>
       </c>
       <c r="B32" s="2">
-        <v>11.1</v>
+        <v>11.14</v>
       </c>
       <c r="C32" s="3">
-        <v>1766</v>
+        <v>1760</v>
       </c>
       <c r="D32" s="4">
-        <v>0.01907</v>
+        <v>0.01893</v>
       </c>
       <c r="E32" s="4">
-        <v>50.6930693069307</v>
+        <v>0.5069306930693069</v>
       </c>
       <c r="F32" s="4">
         <v>0</v>
       </c>
       <c r="G32" s="4">
-        <v>61.98019801980198</v>
+        <v>0.6198019801980198</v>
       </c>
       <c r="H32" s="4">
-        <v>0.214831</v>
+        <v>0.208797</v>
       </c>
       <c r="I32" s="4">
-        <v>72.07920792079207</v>
+        <v>0.7128712871287129</v>
       </c>
       <c r="J32" s="4">
-        <v>0.0348</v>
+        <v>0.03535</v>
       </c>
       <c r="K32" s="4">
-        <v>31.08910891089109</v>
+        <v>0.3128712871287129</v>
       </c>
       <c r="L32" s="3">
-        <v>53.96039603960396</v>
+        <v>0.5381188118811882</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1814,37 +1814,37 @@
         <v>43</v>
       </c>
       <c r="B33" s="2">
-        <v>86.45999999999999</v>
+        <v>84.239</v>
       </c>
       <c r="C33" s="3">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="D33" s="4">
-        <v>1.576531</v>
+        <v>1.531146</v>
       </c>
       <c r="E33" s="4">
-        <v>99.60396039603961</v>
+        <v>0.9960396039603961</v>
       </c>
       <c r="F33" s="4">
-        <v>0.63815</v>
+        <v>0.628494</v>
       </c>
       <c r="G33" s="4">
-        <v>98.81188118811882</v>
+        <v>0.9881188118811882</v>
       </c>
       <c r="H33" s="4">
-        <v>0.604166</v>
+        <v>0.597654</v>
       </c>
       <c r="I33" s="4">
-        <v>99.00990099009901</v>
+        <v>0.9900990099009901</v>
       </c>
       <c r="J33" s="4">
-        <v>0.597903</v>
+        <v>0.590261</v>
       </c>
       <c r="K33" s="4">
-        <v>99.80198019801981</v>
+        <v>0.998019801980198</v>
       </c>
       <c r="L33" s="3">
-        <v>99.30693069306932</v>
+        <v>0.9930693069306931</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1852,37 +1852,37 @@
         <v>44</v>
       </c>
       <c r="B34" s="2">
-        <v>101.72</v>
+        <v>100.02</v>
       </c>
       <c r="C34" s="3">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D34" s="4">
-        <v>0.130853</v>
+        <v>0.129133</v>
       </c>
       <c r="E34" s="4">
-        <v>64.75247524752476</v>
+        <v>0.6435643564356436</v>
       </c>
       <c r="F34" s="4">
-        <v>-0.008545000000000001</v>
+        <v>-0.008229999999999999</v>
       </c>
       <c r="G34" s="4">
-        <v>60.3960396039604</v>
+        <v>0.6059405940594059</v>
       </c>
       <c r="H34" s="4">
-        <v>0.160483</v>
+        <v>0.164396</v>
       </c>
       <c r="I34" s="4">
-        <v>59.6039603960396</v>
+        <v>0.6118811881188119</v>
       </c>
       <c r="J34" s="4">
-        <v>0.11285</v>
+        <v>0.115512</v>
       </c>
       <c r="K34" s="4">
-        <v>72.87128712871286</v>
+        <v>0.7386138613861387</v>
       </c>
       <c r="L34" s="3">
-        <v>64.4059405940594</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1890,37 +1890,37 @@
         <v>45</v>
       </c>
       <c r="B35" s="2">
-        <v>248.08</v>
+        <v>246.17</v>
       </c>
       <c r="C35" s="3">
         <v>79</v>
       </c>
       <c r="D35" s="4">
-        <v>0.305662</v>
+        <v>0.306651</v>
       </c>
       <c r="E35" s="4">
-        <v>80.79207920792079</v>
+        <v>0.807920792079208</v>
       </c>
       <c r="F35" s="4">
-        <v>0.06117</v>
+        <v>0.0588</v>
       </c>
       <c r="G35" s="4">
-        <v>71.88118811881188</v>
+        <v>0.7148514851485149</v>
       </c>
       <c r="H35" s="4">
-        <v>0.025412</v>
+        <v>0.025086</v>
       </c>
       <c r="I35" s="4">
-        <v>22.77227722772277</v>
+        <v>0.2277227722772277</v>
       </c>
       <c r="J35" s="4">
-        <v>-0.04391</v>
+        <v>-0.045294</v>
       </c>
       <c r="K35" s="4">
-        <v>7.128712871287129</v>
+        <v>0.07128712871287129</v>
       </c>
       <c r="L35" s="3">
-        <v>45.64356435643564</v>
+        <v>0.4554455445544555</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1928,37 +1928,37 @@
         <v>46</v>
       </c>
       <c r="B36" s="2">
-        <v>163.34</v>
+        <v>166.87</v>
       </c>
       <c r="C36" s="3">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D36" s="4">
-        <v>0.19125</v>
+        <v>0.19346</v>
       </c>
       <c r="E36" s="4">
-        <v>69.3069306930693</v>
+        <v>0.6990099009900991</v>
       </c>
       <c r="F36" s="4">
-        <v>-0.09439</v>
+        <v>-0.09470000000000001</v>
       </c>
       <c r="G36" s="4">
-        <v>46.33663366336634</v>
+        <v>0.4613861386138614</v>
       </c>
       <c r="H36" s="4">
-        <v>0.28009</v>
+        <v>0.27734</v>
       </c>
       <c r="I36" s="4">
-        <v>84.15841584158416</v>
+        <v>0.8237623762376238</v>
       </c>
       <c r="J36" s="4">
-        <v>0.08018500000000001</v>
+        <v>0.07978300000000001</v>
       </c>
       <c r="K36" s="4">
-        <v>55.04950495049505</v>
+        <v>0.5465346534653466</v>
       </c>
       <c r="L36" s="3">
-        <v>63.71287128712871</v>
+        <v>0.6326732673267327</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1966,37 +1966,37 @@
         <v>47</v>
       </c>
       <c r="B37" s="2">
-        <v>270.34</v>
+        <v>261.217</v>
       </c>
       <c r="C37" s="3">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D37" s="4">
-        <v>0.173079</v>
+        <v>0.172976</v>
       </c>
       <c r="E37" s="4">
-        <v>67.52475247524752</v>
+        <v>0.6732673267326733</v>
       </c>
       <c r="F37" s="4">
-        <v>0.058757</v>
+        <v>0.058386</v>
       </c>
       <c r="G37" s="4">
-        <v>71.28712871287129</v>
+        <v>0.7128712871287129</v>
       </c>
       <c r="H37" s="4">
-        <v>0.08143</v>
+        <v>0.08098</v>
       </c>
       <c r="I37" s="4">
-        <v>36.63366336633663</v>
+        <v>0.3643564356435643</v>
       </c>
       <c r="J37" s="4">
-        <v>-0.027967</v>
+        <v>-0.027592</v>
       </c>
       <c r="K37" s="4">
-        <v>9.108910891089108</v>
+        <v>0.09108910891089109</v>
       </c>
       <c r="L37" s="3">
-        <v>46.13861386138614</v>
+        <v>0.4603960396039604</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2004,37 +2004,37 @@
         <v>48</v>
       </c>
       <c r="B38" s="2">
-        <v>3238.65</v>
+        <v>3304.08</v>
       </c>
       <c r="C38" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38" s="4">
-        <v>0.759162</v>
+        <v>0.73225</v>
       </c>
       <c r="E38" s="4">
-        <v>97.62376237623762</v>
+        <v>0.9762376237623762</v>
       </c>
       <c r="F38" s="4">
-        <v>0.485715</v>
+        <v>0.492282</v>
       </c>
       <c r="G38" s="4">
-        <v>97.22772277227723</v>
+        <v>0.9722772277227724</v>
       </c>
       <c r="H38" s="4">
-        <v>0.338409</v>
+        <v>0.341265</v>
       </c>
       <c r="I38" s="4">
-        <v>90.29702970297029</v>
+        <v>0.904950495049505</v>
       </c>
       <c r="J38" s="4">
-        <v>0.02886</v>
+        <v>0.028314</v>
       </c>
       <c r="K38" s="4">
-        <v>28.71287128712871</v>
+        <v>0.2871287128712872</v>
       </c>
       <c r="L38" s="3">
-        <v>78.46534653465346</v>
+        <v>0.7851485148514852</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2042,37 +2042,37 @@
         <v>49</v>
       </c>
       <c r="B39" s="2">
-        <v>236.6</v>
+        <v>238.423</v>
       </c>
       <c r="C39" s="3">
         <v>82</v>
       </c>
       <c r="D39" s="4">
-        <v>-0.016249</v>
+        <v>-0.015765</v>
       </c>
       <c r="E39" s="4">
-        <v>45.54455445544554</v>
+        <v>0.4554455445544554</v>
       </c>
       <c r="F39" s="4">
-        <v>-0.00709</v>
+        <v>-0.007035</v>
       </c>
       <c r="G39" s="4">
-        <v>60.99009900990099</v>
+        <v>0.6099009900990099</v>
       </c>
       <c r="H39" s="4">
-        <v>0.059367</v>
+        <v>0.061011</v>
       </c>
       <c r="I39" s="4">
-        <v>30.69306930693069</v>
+        <v>0.3089108910891089</v>
       </c>
       <c r="J39" s="4">
-        <v>0.080003</v>
+        <v>0.079803</v>
       </c>
       <c r="K39" s="4">
-        <v>54.85148514851485</v>
+        <v>0.5485148514851486</v>
       </c>
       <c r="L39" s="3">
-        <v>48.01980198019802</v>
+        <v>0.4806930693069307</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2080,37 +2080,37 @@
         <v>50</v>
       </c>
       <c r="B40" s="2">
-        <v>317.65</v>
+        <v>320.72</v>
       </c>
       <c r="C40" s="3">
         <v>61</v>
       </c>
       <c r="D40" s="4">
-        <v>0.490582</v>
+        <v>0.486104</v>
       </c>
       <c r="E40" s="4">
-        <v>91.28712871287129</v>
+        <v>0.9108910891089108</v>
       </c>
       <c r="F40" s="4">
-        <v>0.090221</v>
+        <v>0.094138</v>
       </c>
       <c r="G40" s="4">
-        <v>75.04950495049505</v>
+        <v>0.7544554455445546</v>
       </c>
       <c r="H40" s="4">
-        <v>0.19457</v>
+        <v>0.194556</v>
       </c>
       <c r="I40" s="4">
-        <v>68.91089108910892</v>
+        <v>0.6910891089108911</v>
       </c>
       <c r="J40" s="4">
-        <v>0.03591</v>
+        <v>0.03519</v>
       </c>
       <c r="K40" s="4">
-        <v>31.48514851485148</v>
+        <v>0.3108910891089109</v>
       </c>
       <c r="L40" s="3">
-        <v>66.68316831683168</v>
+        <v>0.6668316831683169</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2118,37 +2118,37 @@
         <v>51</v>
       </c>
       <c r="B41" s="2">
-        <v>280.78</v>
+        <v>284.54</v>
       </c>
       <c r="C41" s="3">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D41" s="4">
-        <v>-0.042092</v>
+        <v>-0.041666</v>
       </c>
       <c r="E41" s="4">
-        <v>42.37623762376238</v>
+        <v>0.4237623762376238</v>
       </c>
       <c r="F41" s="4">
-        <v>0.000404</v>
+        <v>0.000415</v>
       </c>
       <c r="G41" s="4">
-        <v>62.57425742574257</v>
+        <v>0.6257425742574257</v>
       </c>
       <c r="H41" s="4">
-        <v>0.008671999999999999</v>
+        <v>0.008756</v>
       </c>
       <c r="I41" s="4">
-        <v>19.20792079207921</v>
+        <v>0.1920792079207921</v>
       </c>
       <c r="J41" s="4">
-        <v>0.053896</v>
+        <v>0.055455</v>
       </c>
       <c r="K41" s="4">
-        <v>39.00990099009901</v>
+        <v>0.398019801980198</v>
       </c>
       <c r="L41" s="3">
-        <v>40.79207920792079</v>
+        <v>0.4099009900990099</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2156,37 +2156,37 @@
         <v>52</v>
       </c>
       <c r="B42" s="2">
-        <v>200.34</v>
+        <v>197.47</v>
       </c>
       <c r="C42" s="3">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D42" s="4">
-        <v>0.03073</v>
+        <v>0.0304</v>
       </c>
       <c r="E42" s="4">
-        <v>52.47524752475248</v>
+        <v>0.5247524752475248</v>
       </c>
       <c r="F42" s="4">
-        <v>-0.158899</v>
+        <v>-0.161161</v>
       </c>
       <c r="G42" s="4">
-        <v>36.43564356435643</v>
+        <v>0.3584158415841584</v>
       </c>
       <c r="H42" s="4">
-        <v>0.030559</v>
+        <v>0.03052</v>
       </c>
       <c r="I42" s="4">
-        <v>24.15841584158416</v>
+        <v>0.2396039603960396</v>
       </c>
       <c r="J42" s="4">
-        <v>-0.0005330000000000001</v>
+        <v>-0.000531</v>
       </c>
       <c r="K42" s="4">
-        <v>18.41584158415841</v>
+        <v>0.1841584158415842</v>
       </c>
       <c r="L42" s="3">
-        <v>32.87128712871287</v>
+        <v>0.3267326732673267</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2194,37 +2194,37 @@
         <v>53</v>
       </c>
       <c r="B43" s="2">
-        <v>49.01</v>
+        <v>50.9</v>
       </c>
       <c r="C43" s="3">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="D43" s="4">
-        <v>0.067428</v>
+        <v>0.06758699999999999</v>
       </c>
       <c r="E43" s="4">
-        <v>56.03960396039604</v>
+        <v>0.5603960396039603</v>
       </c>
       <c r="F43" s="4">
-        <v>0.142803</v>
+        <v>0.140994</v>
       </c>
       <c r="G43" s="4">
-        <v>81.38613861386139</v>
+        <v>0.8118811881188118</v>
       </c>
       <c r="H43" s="4">
-        <v>0.096371</v>
+        <v>0.09592100000000001</v>
       </c>
       <c r="I43" s="4">
-        <v>40.99009900990099</v>
+        <v>0.4059405940594059</v>
       </c>
       <c r="J43" s="4">
-        <v>0.023223</v>
+        <v>0.023099</v>
       </c>
       <c r="K43" s="4">
-        <v>26.33663366336634</v>
+        <v>0.2613861386138614</v>
       </c>
       <c r="L43" s="3">
-        <v>51.18811881188119</v>
+        <v>0.5099009900990099</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2232,37 +2232,37 @@
         <v>54</v>
       </c>
       <c r="B44" s="2">
-        <v>15.58</v>
+        <v>16.09</v>
       </c>
       <c r="C44" s="3">
-        <v>1258</v>
+        <v>1218</v>
       </c>
       <c r="D44" s="4">
-        <v>-0.318913</v>
+        <v>-0.310509</v>
       </c>
       <c r="E44" s="4">
-        <v>13.46534653465346</v>
+        <v>0.1386138613861386</v>
       </c>
       <c r="F44" s="4">
-        <v>-0.466559</v>
+        <v>-0.454645</v>
       </c>
       <c r="G44" s="4">
-        <v>5.346534653465347</v>
+        <v>0.05544554455445544</v>
       </c>
       <c r="H44" s="4">
-        <v>0.252171</v>
+        <v>0.248582</v>
       </c>
       <c r="I44" s="4">
-        <v>79.4059405940594</v>
+        <v>0.7920792079207921</v>
       </c>
       <c r="J44" s="4">
-        <v>0.189672</v>
+        <v>0.19474</v>
       </c>
       <c r="K44" s="4">
-        <v>93.26732673267327</v>
+        <v>0.9366336633663366</v>
       </c>
       <c r="L44" s="3">
-        <v>47.87128712871287</v>
+        <v>0.4806930693069307</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2270,37 +2270,37 @@
         <v>55</v>
       </c>
       <c r="B45" s="2">
-        <v>294.06</v>
+        <v>289.3</v>
       </c>
       <c r="C45" s="3">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D45" s="4">
-        <v>0.235821</v>
+        <v>0.237723</v>
       </c>
       <c r="E45" s="4">
-        <v>74.85148514851485</v>
+        <v>0.7504950495049505</v>
       </c>
       <c r="F45" s="4">
-        <v>0.121247</v>
+        <v>0.119995</v>
       </c>
       <c r="G45" s="4">
-        <v>79.00990099009901</v>
+        <v>0.7900990099009901</v>
       </c>
       <c r="H45" s="4">
-        <v>0.207192</v>
+        <v>0.211171</v>
       </c>
       <c r="I45" s="4">
-        <v>70.6930693069307</v>
+        <v>0.7188118811881188</v>
       </c>
       <c r="J45" s="4">
-        <v>0.046014</v>
+        <v>0.044402</v>
       </c>
       <c r="K45" s="4">
-        <v>35.44554455445545</v>
+        <v>0.3504950495049505</v>
       </c>
       <c r="L45" s="3">
-        <v>65</v>
+        <v>0.6524752475247525</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2308,37 +2308,37 @@
         <v>56</v>
       </c>
       <c r="B46" s="2">
-        <v>111.77</v>
+        <v>112.89</v>
       </c>
       <c r="C46" s="3">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D46" s="4">
-        <v>0.220571</v>
+        <v>0.21864</v>
       </c>
       <c r="E46" s="4">
-        <v>72.67326732673267</v>
+        <v>0.7267326732673267</v>
       </c>
       <c r="F46" s="4">
-        <v>0.050214</v>
+        <v>0.050554</v>
       </c>
       <c r="G46" s="4">
-        <v>70.6930693069307</v>
+        <v>0.706930693069307</v>
       </c>
       <c r="H46" s="4">
-        <v>0.214841</v>
+        <v>0.210227</v>
       </c>
       <c r="I46" s="4">
-        <v>72.27722772277228</v>
+        <v>0.7168316831683168</v>
       </c>
       <c r="J46" s="4">
-        <v>0.140396</v>
+        <v>0.139163</v>
       </c>
       <c r="K46" s="4">
-        <v>82.77227722772277</v>
+        <v>0.8257425742574257</v>
       </c>
       <c r="L46" s="3">
-        <v>74.60396039603961</v>
+        <v>0.7440594059405941</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2346,37 +2346,37 @@
         <v>57</v>
       </c>
       <c r="B47" s="2">
-        <v>85.14</v>
+        <v>88.59999999999999</v>
       </c>
       <c r="C47" s="3">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D47" s="4">
-        <v>-0.019219</v>
+        <v>-0.019179</v>
       </c>
       <c r="E47" s="4">
-        <v>45.34653465346535</v>
+        <v>0.4534653465346535</v>
       </c>
       <c r="F47" s="4">
-        <v>-0.040899</v>
+        <v>-0.039621</v>
       </c>
       <c r="G47" s="4">
-        <v>55.04950495049505</v>
+        <v>0.5524752475247525</v>
       </c>
       <c r="H47" s="4">
-        <v>0.240282</v>
+        <v>0.231802</v>
       </c>
       <c r="I47" s="4">
-        <v>76.83168316831683</v>
+        <v>0.7584158415841584</v>
       </c>
       <c r="J47" s="4">
-        <v>0.095252</v>
+        <v>0.095571</v>
       </c>
       <c r="K47" s="4">
-        <v>64.75247524752476</v>
+        <v>0.6534653465346534</v>
       </c>
       <c r="L47" s="3">
-        <v>60.49504950495049</v>
+        <v>0.6044554455445544</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -2384,37 +2384,37 @@
         <v>58</v>
       </c>
       <c r="B48" s="2">
-        <v>177.06</v>
+        <v>180.25</v>
       </c>
       <c r="C48" s="3">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D48" s="4">
-        <v>0.207608</v>
+        <v>0.200601</v>
       </c>
       <c r="E48" s="4">
-        <v>72.27722772277228</v>
+        <v>0.7168316831683168</v>
       </c>
       <c r="F48" s="4">
-        <v>0.030437</v>
+        <v>0.030712</v>
       </c>
       <c r="G48" s="4">
-        <v>67.52475247524752</v>
+        <v>0.6752475247524753</v>
       </c>
       <c r="H48" s="4">
-        <v>0.159048</v>
+        <v>0.155758</v>
       </c>
       <c r="I48" s="4">
-        <v>59.20792079207921</v>
+        <v>0.5841584158415841</v>
       </c>
       <c r="J48" s="4">
-        <v>0.09536799999999999</v>
+        <v>0.092513</v>
       </c>
       <c r="K48" s="4">
-        <v>64.95049504950495</v>
+        <v>0.6336633663366337</v>
       </c>
       <c r="L48" s="3">
-        <v>65.99009900990099</v>
+        <v>0.6524752475247525</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -2422,37 +2422,37 @@
         <v>59</v>
       </c>
       <c r="B49" s="2">
-        <v>110.56</v>
+        <v>109.01</v>
       </c>
       <c r="C49" s="3">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D49" s="4">
-        <v>-0.035137</v>
+        <v>-0.034199</v>
       </c>
       <c r="E49" s="4">
-        <v>43.16831683168317</v>
+        <v>0.4316831683168317</v>
       </c>
       <c r="F49" s="4">
-        <v>-0.1065</v>
+        <v>-0.1112</v>
       </c>
       <c r="G49" s="4">
-        <v>43.96039603960396</v>
+        <v>0.4356435643564357</v>
       </c>
       <c r="H49" s="4">
-        <v>0.089653</v>
+        <v>0.08760900000000001</v>
       </c>
       <c r="I49" s="4">
-        <v>39.00990099009901</v>
+        <v>0.3821782178217822</v>
       </c>
       <c r="J49" s="4">
-        <v>0.063884</v>
+        <v>0.06393</v>
       </c>
       <c r="K49" s="4">
-        <v>46.13861386138614</v>
+        <v>0.4653465346534654</v>
       </c>
       <c r="L49" s="3">
-        <v>43.06930693069307</v>
+        <v>0.4287128712871288</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -2460,37 +2460,37 @@
         <v>60</v>
       </c>
       <c r="B50" s="2">
-        <v>84.11</v>
+        <v>87.41</v>
       </c>
       <c r="C50" s="3">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D50" s="4">
-        <v>0.704282</v>
+        <v>0.690043</v>
       </c>
       <c r="E50" s="4">
-        <v>97.42574257425743</v>
+        <v>0.9742574257425742</v>
       </c>
       <c r="F50" s="4">
-        <v>0.351524</v>
+        <v>0.354006</v>
       </c>
       <c r="G50" s="4">
-        <v>95.04950495049505</v>
+        <v>0.9504950495049505</v>
       </c>
       <c r="H50" s="4">
-        <v>0.133808</v>
+        <v>0.130251</v>
       </c>
       <c r="I50" s="4">
-        <v>52.27722772277227</v>
+        <v>0.5089108910891089</v>
       </c>
       <c r="J50" s="4">
-        <v>0.041082</v>
+        <v>0.040945</v>
       </c>
       <c r="K50" s="4">
-        <v>34.25742574257426</v>
+        <v>0.3405940594059406</v>
       </c>
       <c r="L50" s="3">
-        <v>69.75247524752476</v>
+        <v>0.6935643564356435</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -2498,37 +2498,37 @@
         <v>61</v>
       </c>
       <c r="B51" s="2">
-        <v>161.22</v>
+        <v>160</v>
       </c>
       <c r="C51" s="3">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D51" s="4">
-        <v>-0.258126</v>
+        <v>-0.26325</v>
       </c>
       <c r="E51" s="4">
-        <v>20.79207920792079</v>
+        <v>0.203960396039604</v>
       </c>
       <c r="F51" s="4">
-        <v>-0.309778</v>
+        <v>-0.319747</v>
       </c>
       <c r="G51" s="4">
-        <v>17.42574257425743</v>
+        <v>0.1643564356435644</v>
       </c>
       <c r="H51" s="4">
-        <v>-0.0633</v>
+        <v>-0.0624</v>
       </c>
       <c r="I51" s="4">
-        <v>6.930693069306931</v>
+        <v>0.06930693069306931</v>
       </c>
       <c r="J51" s="4">
-        <v>0.003748</v>
+        <v>0.003684</v>
       </c>
       <c r="K51" s="4">
-        <v>19.8019801980198</v>
+        <v>0.196039603960396</v>
       </c>
       <c r="L51" s="3">
-        <v>16.23762376237624</v>
+        <v>0.1584158415841584</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -2536,37 +2536,37 @@
         <v>62</v>
       </c>
       <c r="B52" s="2">
-        <v>326.28</v>
+        <v>325.95</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D52" s="4">
-        <v>0.20632</v>
+        <v>0.208469</v>
       </c>
       <c r="E52" s="4">
-        <v>72.07920792079207</v>
+        <v>0.7227722772277229</v>
       </c>
       <c r="F52" s="4">
-        <v>0.03788</v>
+        <v>0.038683</v>
       </c>
       <c r="G52" s="4">
-        <v>68.71287128712871</v>
+        <v>0.6891089108910892</v>
       </c>
       <c r="H52" s="4">
-        <v>0.186333</v>
+        <v>0.185981</v>
       </c>
       <c r="I52" s="4">
-        <v>67.92079207920793</v>
+        <v>0.6752475247524753</v>
       </c>
       <c r="J52" s="4">
-        <v>0.020587</v>
+        <v>0.020828</v>
       </c>
       <c r="K52" s="4">
-        <v>25.54455445544555</v>
+        <v>0.2554455445544555</v>
       </c>
       <c r="L52" s="3">
-        <v>58.56435643564356</v>
+        <v>0.5856435643564357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>